<commit_message>
Sorts formulae by depth
</commit_message>
<xml_diff>
--- a/checker.xlsx
+++ b/checker.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markfa\Dropbox\OLM\Products\Calc Engine\Releases\2.0\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Mark\Projects\ExCell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,10 +16,7 @@
     <sheet name="Calculation" sheetId="3" r:id="rId2"/>
     <sheet name="Text" sheetId="4" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="NEEDS">Calculation!$B$3</definedName>
-  </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -269,7 +266,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Score</t>
   </si>
@@ -434,11 +431,14 @@
   <si>
     <t>Text4</t>
   </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,6 +714,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -749,6 +766,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -925,6 +959,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -968,73 +1003,119 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
@@ -1055,10 +1136,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>VLOOKUP(B2,K2:L4,2,FALSE)</f>
+        <f>VLOOKUP(B2,K2:L3,2,FALSE)</f>
         <v>0</v>
       </c>
       <c r="E2" t="s">
@@ -1117,13 +1199,22 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="10">
-        <f>IF(IFERROR(SEARCH("0", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("0", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C4">
@@ -1135,15 +1226,6 @@
       </c>
       <c r="G4">
         <v>4</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1151,11 +1233,11 @@
         <v>14</v>
       </c>
       <c r="B5" s="10">
-        <f>IF(IFERROR(SEARCH("1", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("1", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C13" si="0">IF(B5&gt;0,10,0)</f>
+        <f>IF(B5&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F5">
@@ -1170,11 +1252,11 @@
         <v>15</v>
       </c>
       <c r="B6" s="10">
-        <f>IF(IFERROR(SEARCH("2", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("2", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f>IF(B6&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F6">
@@ -1192,11 +1274,11 @@
         <v>16</v>
       </c>
       <c r="B7" s="10">
-        <f>IF(IFERROR(SEARCH("3", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("3", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f>IF(B7&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F7">
@@ -1211,11 +1293,11 @@
         <v>17</v>
       </c>
       <c r="B8" s="10">
-        <f>IF(IFERROR(SEARCH("4", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("4", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f>IF(B8&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F8">
@@ -1230,11 +1312,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="10">
-        <f>IF(IFERROR(SEARCH("5", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("5", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f>IF(B9&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F9">
@@ -1249,11 +1331,11 @@
         <v>19</v>
       </c>
       <c r="B10" s="10">
-        <f>IF(IFERROR(SEARCH("6", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("6", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f>IF(B10&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F10">
@@ -1268,11 +1350,11 @@
         <v>20</v>
       </c>
       <c r="B11" s="10">
-        <f>IF(IFERROR(SEARCH("7", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("7", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f>IF(B11&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F11">
@@ -1287,11 +1369,11 @@
         <v>21</v>
       </c>
       <c r="B12" s="10">
-        <f>IF(IFERROR(SEARCH("8", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("8", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f>IF(B12&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F12">
@@ -1306,11 +1388,11 @@
         <v>22</v>
       </c>
       <c r="B13" s="10">
-        <f>IF(IFERROR(SEARCH("9", NEEDS), 0),1,0)</f>
+        <f>IF(IFERROR(SEARCH("9", Calculation!$B$3), 0),1,0)</f>
         <v>0</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f>IF(B13&gt;0,10,0)</f>
         <v>0</v>
       </c>
       <c r="F13">
@@ -1408,6 +1490,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">

</xml_diff>